<commit_message>
Implemented passing authentication via the request headers
</commit_message>
<xml_diff>
--- a/resources/API_Doc.xlsx
+++ b/resources/API_Doc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>API_ENDPOINT</t>
   </si>
@@ -35,16 +35,48 @@
   </si>
   <si>
     <t>Login API</t>
+  </si>
+  <si>
+    <t>Create Hospital</t>
+  </si>
+  <si>
+    <t>http://ramsayportalapi-uat.azurewebsites.net/api/hospitals/create</t>
+  </si>
+  <si>
+    <t>{
+ "HospitalId":#hospitalId,
+ "HospitalName":"#hospitalName",
+ "Address1":"dddd",
+ "Address2":"ddddd",
+ "Suburb":"adf",
+ "Web":"tyntymtwym",
+ "SiteCode":"ddd",
+ "Postcode":1,
+ "State":"ddd",
+ "AdminEmail":"sdcs@hadvc.com",
+ "Longitude":0,
+ "Latitude":0,
+ "IsActive":true,
+ "CreateUser":"portaladmin"
+}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -67,16 +99,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -413,24 +450,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
@@ -441,15 +478,29 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Setup script added. Modified project
</commit_message>
<xml_diff>
--- a/resources/API_Doc.xlsx
+++ b/resources/API_Doc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>API_ENDPOINT</t>
   </si>
@@ -59,6 +59,9 @@
  "IsActive":true,
  "CreateUser":"portaladmin"
 }</t>
+  </si>
+  <si>
+    <t>Get Bucket List</t>
   </si>
 </sst>
 </file>
@@ -116,8 +119,36 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -450,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,6 +527,11 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>

</xml_diff>